<commit_message>
suppressed lightning alerts from Imuruk Lake and Ingakslugwat Hills
</commit_message>
<xml_diff>
--- a/alarm_aux_files/volcano_list.xlsx
+++ b/alarm_aux_files/volcano_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10312"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10719"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awech-local/Library/Caches/com.binarynights.ForkLift-3/FileCache/598DAD8A-5ED2-410D-A3CE-E05277D5FFD5/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/awech-local/Library/Caches/com.binarynights.ForkLift-3/FileCache/73361385-523E-4DFA-AD46-35E7B2E9E840/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{967626E7-5B12-344D-A326-1D0D8063FEC1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE2B5C21-D256-D44F-984A-699D7A1F8E6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38380" yWindow="500" windowWidth="31740" windowHeight="21040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Query1" sheetId="1" r:id="rId1"/>
@@ -1449,7 +1449,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1484,7 +1484,8 @@
     <xf numFmtId="1" fontId="1" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="1" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1516,9 +1517,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1556,9 +1557,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1591,26 +1592,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1643,26 +1627,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1839,8 +1806,8 @@
   <dimension ref="A1:M159"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A119" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K150" sqref="K150"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2546,8 +2513,8 @@
       <c r="J17" s="5" t="s">
         <v>368</v>
       </c>
-      <c r="K17" s="5" t="s">
-        <v>368</v>
+      <c r="K17" s="8" t="s">
+        <v>369</v>
       </c>
       <c r="L17" s="5" t="s">
         <v>368</v>
@@ -2557,14 +2524,14 @@
       </c>
     </row>
     <row r="18" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A18" s="1" t="s">
+      <c r="A18" s="4" t="s">
         <v>48</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C18" s="8">
-        <v>314050</v>
+        <v>314030</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>48</v>
@@ -3384,7 +3351,7 @@
         <v>98</v>
       </c>
       <c r="C38" s="8">
-        <v>314030</v>
+        <v>314050</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>99</v>
@@ -7600,19 +7567,20 @@
       </c>
     </row>
     <row r="141" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A141" t="s">
+      <c r="A141" s="12" t="s">
         <v>372</v>
       </c>
-      <c r="B141" t="s">
+      <c r="B141" s="12" t="s">
         <v>373</v>
       </c>
-      <c r="C141" s="12">
+      <c r="C141" s="13">
         <v>284160</v>
       </c>
-      <c r="E141">
+      <c r="D141" s="12"/>
+      <c r="E141" s="12">
         <v>18.77</v>
       </c>
-      <c r="F141">
+      <c r="F141" s="12">
         <v>145.66999999999999</v>
       </c>
       <c r="G141" s="8" t="s">
@@ -7638,19 +7606,20 @@
       </c>
     </row>
     <row r="142" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A142" t="s">
+      <c r="A142" s="12" t="s">
         <v>397</v>
       </c>
-      <c r="B142" t="s">
+      <c r="B142" s="12" t="s">
         <v>398</v>
       </c>
-      <c r="C142" s="12">
+      <c r="C142" s="13">
         <v>284170</v>
       </c>
-      <c r="E142">
+      <c r="D142" s="12"/>
+      <c r="E142" s="12">
         <v>18.13</v>
       </c>
-      <c r="F142">
+      <c r="F142" s="12">
         <v>145.80000000000001</v>
       </c>
       <c r="G142" s="8" t="s">
@@ -7676,19 +7645,20 @@
       </c>
     </row>
     <row r="143" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A143" t="s">
+      <c r="A143" s="12" t="s">
         <v>399</v>
       </c>
-      <c r="B143" t="s">
+      <c r="B143" s="12" t="s">
         <v>400</v>
       </c>
-      <c r="C143" s="12">
+      <c r="C143" s="13">
         <v>284202</v>
       </c>
-      <c r="E143">
+      <c r="D143" s="12"/>
+      <c r="E143" s="12">
         <v>15.62</v>
       </c>
-      <c r="F143">
+      <c r="F143" s="12">
         <v>145.57</v>
       </c>
       <c r="G143" s="8" t="s">
@@ -7714,19 +7684,20 @@
       </c>
     </row>
     <row r="144" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A144" t="s">
+      <c r="A144" s="12" t="s">
         <v>401</v>
       </c>
-      <c r="B144" t="s">
+      <c r="B144" s="12" t="s">
         <v>402</v>
       </c>
-      <c r="C144" s="12">
+      <c r="C144" s="13">
         <v>284192</v>
       </c>
-      <c r="E144">
+      <c r="D144" s="12"/>
+      <c r="E144" s="12">
         <v>16.707999999999998</v>
       </c>
-      <c r="F144">
+      <c r="F144" s="12">
         <v>145.78</v>
       </c>
       <c r="G144" s="8" t="s">
@@ -7752,19 +7723,20 @@
       </c>
     </row>
     <row r="145" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A145" t="s">
+      <c r="A145" s="12" t="s">
         <v>404</v>
       </c>
-      <c r="B145" t="s">
+      <c r="B145" s="12" t="s">
         <v>405</v>
       </c>
-      <c r="C145" s="12">
+      <c r="C145" s="13">
         <v>284142</v>
       </c>
-      <c r="E145">
+      <c r="D145" s="12"/>
+      <c r="E145" s="12">
         <v>20.13</v>
       </c>
-      <c r="F145">
+      <c r="F145" s="12">
         <v>145.1</v>
       </c>
       <c r="G145" s="8" t="s">
@@ -7790,19 +7762,20 @@
       </c>
     </row>
     <row r="146" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A146" t="s">
+      <c r="A146" s="12" t="s">
         <v>382</v>
       </c>
-      <c r="B146" t="s">
+      <c r="B146" s="12" t="s">
         <v>383</v>
       </c>
-      <c r="C146" s="12">
+      <c r="C146" s="13">
         <v>284137</v>
       </c>
-      <c r="E146">
+      <c r="D146" s="12"/>
+      <c r="E146" s="12">
         <v>21.324000000000002</v>
       </c>
-      <c r="F146">
+      <c r="F146" s="12">
         <v>144.19399999999999</v>
       </c>
       <c r="G146" s="8" t="s">
@@ -7828,19 +7801,20 @@
       </c>
     </row>
     <row r="147" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A147" t="s">
+      <c r="A147" s="12" t="s">
         <v>384</v>
       </c>
-      <c r="B147" t="s">
+      <c r="B147" s="12" t="s">
         <v>385</v>
       </c>
-      <c r="C147" s="12">
+      <c r="C147" s="13">
         <v>284201</v>
       </c>
-      <c r="E147">
+      <c r="D147" s="12"/>
+      <c r="E147" s="12">
         <v>15.93</v>
       </c>
-      <c r="F147">
+      <c r="F147" s="12">
         <v>145.66999999999999</v>
       </c>
       <c r="G147" s="8" t="s">
@@ -7866,19 +7840,20 @@
       </c>
     </row>
     <row r="148" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A148" t="s">
+      <c r="A148" s="12" t="s">
         <v>409</v>
       </c>
-      <c r="B148" t="s">
+      <c r="B148" s="12" t="s">
         <v>390</v>
       </c>
-      <c r="C148" s="12">
+      <c r="C148" s="13">
         <v>284133</v>
       </c>
-      <c r="E148">
+      <c r="D148" s="12"/>
+      <c r="E148" s="12">
         <v>21.93</v>
       </c>
-      <c r="F148">
+      <c r="F148" s="12">
         <v>143.47</v>
       </c>
       <c r="G148" s="8" t="s">
@@ -7904,19 +7879,20 @@
       </c>
     </row>
     <row r="149" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A149" t="s">
+      <c r="A149" s="12" t="s">
         <v>393</v>
       </c>
-      <c r="B149" t="s">
+      <c r="B149" s="12" t="s">
         <v>394</v>
       </c>
-      <c r="C149" s="12">
+      <c r="C149" s="13">
         <v>284135</v>
       </c>
-      <c r="E149">
+      <c r="D149" s="12"/>
+      <c r="E149" s="12">
         <v>21.6</v>
       </c>
-      <c r="F149">
+      <c r="F149" s="12">
         <v>143.637</v>
       </c>
       <c r="G149" s="8" t="s">
@@ -7942,19 +7918,20 @@
       </c>
     </row>
     <row r="150" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A150" t="s">
+      <c r="A150" s="12" t="s">
         <v>408</v>
       </c>
-      <c r="B150" t="s">
+      <c r="B150" s="12" t="s">
         <v>403</v>
       </c>
-      <c r="C150" s="12">
+      <c r="C150" s="13">
         <v>284193</v>
       </c>
-      <c r="E150">
+      <c r="D150" s="12"/>
+      <c r="E150" s="12">
         <v>16.579999999999998</v>
       </c>
-      <c r="F150">
+      <c r="F150" s="12">
         <v>145.78</v>
       </c>
       <c r="G150" s="8" t="s">
@@ -7980,19 +7957,20 @@
       </c>
     </row>
     <row r="151" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A151" t="s">
+      <c r="A151" s="12" t="s">
         <v>406</v>
       </c>
-      <c r="B151" t="s">
+      <c r="B151" s="12" t="s">
         <v>407</v>
       </c>
-      <c r="C151" s="12">
+      <c r="C151" s="13">
         <v>284191</v>
       </c>
-      <c r="E151">
+      <c r="D151" s="12"/>
+      <c r="E151" s="12">
         <v>16.88</v>
       </c>
-      <c r="F151">
+      <c r="F151" s="12">
         <v>145.85</v>
       </c>
       <c r="G151" s="8" t="s">
@@ -8018,19 +7996,20 @@
       </c>
     </row>
     <row r="152" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A152" t="s">
+      <c r="A152" s="12" t="s">
         <v>374</v>
       </c>
-      <c r="B152" t="s">
+      <c r="B152" s="12" t="s">
         <v>375</v>
       </c>
-      <c r="C152" s="12">
+      <c r="C152" s="13">
         <v>284141</v>
       </c>
-      <c r="E152">
+      <c r="D152" s="12"/>
+      <c r="E152" s="12">
         <v>20.420000000000002</v>
       </c>
-      <c r="F152">
+      <c r="F152" s="12">
         <v>145.03</v>
       </c>
       <c r="G152" s="8" t="s">
@@ -8056,19 +8035,20 @@
       </c>
     </row>
     <row r="153" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A153" t="s">
+      <c r="A153" s="12" t="s">
         <v>376</v>
       </c>
-      <c r="B153" t="s">
+      <c r="B153" s="12" t="s">
         <v>377</v>
       </c>
-      <c r="C153" s="12">
+      <c r="C153" s="13">
         <v>284180</v>
       </c>
-      <c r="E153">
+      <c r="D153" s="12"/>
+      <c r="E153" s="12">
         <v>17.600000000000001</v>
       </c>
-      <c r="F153">
+      <c r="F153" s="12">
         <v>145.83000000000001</v>
       </c>
       <c r="G153" s="8" t="s">
@@ -8094,19 +8074,20 @@
       </c>
     </row>
     <row r="154" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A154" t="s">
+      <c r="A154" s="12" t="s">
         <v>378</v>
       </c>
-      <c r="B154" t="s">
+      <c r="B154" s="12" t="s">
         <v>379</v>
       </c>
-      <c r="C154" s="12">
+      <c r="C154" s="13">
         <v>284200</v>
       </c>
-      <c r="E154">
+      <c r="D154" s="12"/>
+      <c r="E154" s="12">
         <v>16.350000000000001</v>
       </c>
-      <c r="F154">
+      <c r="F154" s="12">
         <v>145.66999999999999</v>
       </c>
       <c r="G154" s="8" t="s">
@@ -8132,19 +8113,20 @@
       </c>
     </row>
     <row r="155" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A155" t="s">
+      <c r="A155" s="12" t="s">
         <v>380</v>
       </c>
-      <c r="B155" t="s">
+      <c r="B155" s="12" t="s">
         <v>381</v>
       </c>
-      <c r="C155" s="12">
+      <c r="C155" s="13">
         <v>284150</v>
       </c>
-      <c r="E155">
+      <c r="D155" s="12"/>
+      <c r="E155" s="12">
         <v>19.670000000000002</v>
       </c>
-      <c r="F155">
+      <c r="F155" s="12">
         <v>145.4</v>
       </c>
       <c r="G155" s="8" t="s">
@@ -8170,19 +8152,20 @@
       </c>
     </row>
     <row r="156" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A156" t="s">
+      <c r="A156" s="12" t="s">
         <v>386</v>
       </c>
-      <c r="B156" t="s">
+      <c r="B156" s="12" t="s">
         <v>387</v>
       </c>
-      <c r="C156" s="12">
+      <c r="C156" s="13">
         <v>284210</v>
       </c>
-      <c r="E156">
+      <c r="D156" s="12"/>
+      <c r="E156" s="12">
         <v>15</v>
       </c>
-      <c r="F156">
+      <c r="F156" s="12">
         <v>145.25</v>
       </c>
       <c r="G156" s="8" t="s">
@@ -8208,19 +8191,20 @@
       </c>
     </row>
     <row r="157" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A157" t="s">
+      <c r="A157" s="12" t="s">
         <v>388</v>
       </c>
-      <c r="B157" t="s">
+      <c r="B157" s="12" t="s">
         <v>389</v>
       </c>
-      <c r="C157" s="12">
+      <c r="C157" s="13">
         <v>284140</v>
       </c>
-      <c r="E157">
+      <c r="D157" s="12"/>
+      <c r="E157" s="12">
         <v>20.53</v>
       </c>
-      <c r="F157">
+      <c r="F157" s="12">
         <v>144.9</v>
       </c>
       <c r="G157" s="8" t="s">
@@ -8246,19 +8230,20 @@
       </c>
     </row>
     <row r="158" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A158" t="s">
+      <c r="A158" s="12" t="s">
         <v>391</v>
       </c>
-      <c r="B158" t="s">
+      <c r="B158" s="12" t="s">
         <v>392</v>
       </c>
-      <c r="C158" s="12">
+      <c r="C158" s="13">
         <v>284190</v>
       </c>
-      <c r="E158">
+      <c r="D158" s="12"/>
+      <c r="E158" s="12">
         <v>17.32</v>
       </c>
-      <c r="F158">
+      <c r="F158" s="12">
         <v>145.85</v>
       </c>
       <c r="G158" s="8" t="s">
@@ -8284,19 +8269,20 @@
       </c>
     </row>
     <row r="159" spans="1:13" ht="16" x14ac:dyDescent="0.2">
-      <c r="A159" t="s">
+      <c r="A159" s="12" t="s">
         <v>395</v>
       </c>
-      <c r="B159" t="s">
+      <c r="B159" s="12" t="s">
         <v>396</v>
       </c>
-      <c r="C159" s="12">
+      <c r="C159" s="13">
         <v>284143</v>
       </c>
-      <c r="E159">
+      <c r="D159" s="12"/>
+      <c r="E159" s="12">
         <v>20.02</v>
       </c>
-      <c r="F159">
+      <c r="F159" s="12">
         <v>145.22</v>
       </c>
       <c r="G159" s="8" t="s">

</xml_diff>